<commit_message>
added banana to barrel plug adapter to purchase request form
</commit_message>
<xml_diff>
--- a/manufacturing/purchase-form.xlsx
+++ b/manufacturing/purchase-form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t xml:space="preserve">Breadboard Power Supply</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t xml:space="preserve">IC REG LIN POS ADJ 500MA SOT223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banana to barrel plug cable (2-pack)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/PNGKNYOCN-Banana-Bullet-Plug18AWG-Connector/dp/B0BC1LXMG4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC 5.5mm x 2.1mm to 4mm Banana Plugs Cable</t>
   </si>
   <si>
     <t xml:space="preserve">Totals:</t>
@@ -418,7 +430,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,10 +468,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -772,21 +780,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:H50"/>
+  <dimension ref="A2:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="75.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="79.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40.77"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,10 +850,10 @@
         <f aca="false">D4*E4</f>
         <v>123</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -870,13 +878,13 @@
       <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -895,7 +903,7 @@
       <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -920,7 +928,7 @@
       <c r="G7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -945,7 +953,7 @@
       <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -970,7 +978,7 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -995,7 +1003,7 @@
       <c r="G10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1020,7 +1028,7 @@
       <c r="G11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1045,7 +1053,7 @@
       <c r="G12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1070,7 +1078,7 @@
       <c r="G13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1095,7 +1103,7 @@
       <c r="G14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1120,7 +1128,7 @@
       <c r="G15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1145,7 +1153,7 @@
       <c r="G16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1170,7 +1178,7 @@
       <c r="G17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1195,129 +1203,117 @@
       <c r="G18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9" t="n">
+      <c r="B19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="15" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="F19" s="16" t="n">
         <f aca="false">D19*E19</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="11"/>
+        <v>32.97</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9" t="n">
-        <f aca="false">D20*E20</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17" t="n">
-        <f aca="false">D21*E21</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
+      <c r="B20" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20" t="n">
+        <f aca="false">SUM(E4:E19)</f>
+        <v>26.485</v>
+      </c>
+      <c r="F20" s="20" t="n">
+        <f aca="false">SUM(F4:F19)</f>
+        <v>417.034</v>
+      </c>
+      <c r="G20" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21" t="n">
-        <f aca="false">SUM(E4:E21)</f>
-        <v>15.495</v>
-      </c>
-      <c r="F22" s="21" t="n">
-        <f aca="false">SUM(F4:F21)</f>
-        <v>384.064</v>
-      </c>
-      <c r="G22" s="22"/>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="23"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="23"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="23"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="23"/>
+      <c r="D27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="23"/>
+      <c r="D28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="23"/>
+      <c r="D29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="23"/>
+      <c r="D30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="23"/>
+      <c r="D31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="23"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="23"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="23"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="23"/>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="24"/>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="22"/>
+      <c r="F45" s="23"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E46" s="23"/>
-      <c r="F46" s="24"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="23"/>
-      <c r="F47" s="24"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="23"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="23"/>
-      <c r="F48" s="24"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="23"/>
-      <c r="F49" s="24"/>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="23"/>
-      <c r="F50" s="24"/>
-    </row>
+      <c r="E48" s="22"/>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" display="https://oshpark.com/"/>
@@ -1335,6 +1331,7 @@
     <hyperlink ref="G16" r:id="rId13" display="https://www.digikey.com/en/products/detail/e-switch/EG1271/251335"/>
     <hyperlink ref="G17" r:id="rId14" display="https://www.digikey.com/en/products/detail/e-switch/EG2315/101778"/>
     <hyperlink ref="G18" r:id="rId15" display="https://www.digikey.com/en/products/detail/texas-instruments/LM317MDCYR/454187"/>
+    <hyperlink ref="G19" r:id="rId16" display="https://www.amazon.com/PNGKNYOCN-Banana-Bullet-Plug18AWG-Connector/dp/B0BC1LXMG4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>